<commit_message>
fixed dip switch tables
</commit_message>
<xml_diff>
--- a/Documents/4&6 Digit Ethernet Display Commands.xlsx
+++ b/Documents/4&6 Digit Ethernet Display Commands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrmachado\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrmachado\Documents\GitHub\ADP_Resources\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00652A7-A026-42D9-9834-B7B2EC0520F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1FFC11-A044-4D16-B731-C69E6616D44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28950" yWindow="-8730" windowWidth="28575" windowHeight="31500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41010" yWindow="-4440" windowWidth="28575" windowHeight="22710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4 Digit Ethernet Display Comman" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="102">
   <si>
     <t>&lt;0x01&gt;Z00&lt;0x02&gt;G11234&lt;0x04&gt;</t>
   </si>
@@ -251,24 +251,6 @@
     <t xml:space="preserve">Value if ON </t>
   </si>
   <si>
-    <t>8 Hour Modification On</t>
-  </si>
-  <si>
-    <t>8 Hour Modification Off</t>
-  </si>
-  <si>
-    <t>4 Hour Modification On</t>
-  </si>
-  <si>
-    <t>4 Hour Modification Off</t>
-  </si>
-  <si>
-    <t>2 Hour Modification On</t>
-  </si>
-  <si>
-    <t>1 Hour Modification On</t>
-  </si>
-  <si>
     <t>SW 6 ON</t>
   </si>
   <si>
@@ -321,6 +303,30 @@
   </si>
   <si>
     <t>hh:mm</t>
+  </si>
+  <si>
+    <t>2 Hour Modification OFF</t>
+  </si>
+  <si>
+    <t>1 Hour Modification OFF</t>
+  </si>
+  <si>
+    <t>8 Hour Modification OFF</t>
+  </si>
+  <si>
+    <t>4 Hour Modification OFF</t>
+  </si>
+  <si>
+    <t>8 Hour Modification ON</t>
+  </si>
+  <si>
+    <t>4 Hour Modification ON</t>
+  </si>
+  <si>
+    <t>2 Hour Modification ON</t>
+  </si>
+  <si>
+    <t>1 Hour Modification ON</t>
   </si>
 </sst>
 </file>
@@ -820,7 +826,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -829,7 +835,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1517,7 +1522,7 @@
   <dimension ref="B2:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J12"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,13 +1535,13 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>97</v>
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -1555,10 +1560,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -1566,10 +1571,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -1577,10 +1582,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -1588,10 +1593,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -1599,10 +1604,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -1610,10 +1615,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -1621,10 +1626,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
@@ -1632,21 +1637,21 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
+      </c>
+      <c r="D13" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
@@ -1665,10 +1670,10 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
@@ -1676,10 +1681,10 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -1687,10 +1692,10 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -1698,10 +1703,10 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -1709,10 +1714,10 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -1720,10 +1725,10 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -1731,7 +1736,7 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D21" t="s">
         <v>70</v>
@@ -1742,18 +1747,18 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D24" s="3"/>
     </row>
@@ -1784,10 +1789,10 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -1795,10 +1800,10 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -1806,10 +1811,10 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -1817,10 +1822,10 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -1828,10 +1833,10 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -1839,10 +1844,10 @@
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -1850,10 +1855,10 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>